<commit_message>
Began to impliment the LED handling software
</commit_message>
<xml_diff>
--- a/LED Cube Shopping list.xlsx
+++ b/LED Cube Shopping list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wild/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wild/Documents/Projects/trackellite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90F737F-D3F1-C64A-A694-BB69B3FD6E3E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A262E69-38F3-4245-A5C5-15A51A53033B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{4821D1B7-1E32-564A-9100-CE974E243A21}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Shopping list for LED cube</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Part Name</t>
   </si>
   <si>
@@ -48,45 +45,21 @@
     <t>Unit cost</t>
   </si>
   <si>
-    <t>Need</t>
-  </si>
-  <si>
     <t>Total part cost</t>
   </si>
   <si>
-    <t>Blue LED</t>
-  </si>
-  <si>
-    <t>https://www.ebay.co.uk/itm/Ultra-Bright-1-8mm-3mm-5mm-8mm-10mm-Waterclear-LED-Lights/262567656017?hash=item3d22407a51:m:mP-rbIeS38JpaPrfkTbvhbQ</t>
-  </si>
-  <si>
-    <t>330 resistor</t>
-  </si>
-  <si>
     <t>https://www.ebay.co.uk/itm/Resistor-Metal-Film-1-4W-0-25W-5-10-200-270-470-1k-3-3k-10k-20k-47k-Ohm/382625214567?hash=item59163d7067:m:msYdoHTiPmHJqz_OMMrQp8Q&amp;var=651378842494</t>
   </si>
   <si>
-    <t>GPIO pins</t>
-  </si>
-  <si>
     <t>Heat Shrink</t>
   </si>
   <si>
     <t>https://www.ebay.co.uk/itm/Heat-Shrink-2-1-Tube-Tubing-Sleeve-Sleeving-Heat-Shrink-All-Colours-and-Sizes/261960089592?hash=item3cfe09bff8:m:m_EwYaXKVhKo0WUxKvmODIA</t>
   </si>
   <si>
-    <t>Switch</t>
-  </si>
-  <si>
     <t>https://www.ebay.co.uk/itm/illuminated-LED-Toggle-Switch-With-Missile-Style-Flick-Cover-12V-Car-Dash/282258203997?hash=item41b7e6655d:m:mL95Oa7ssQttGbXRMt0rJ9A&amp;var=581300324809</t>
   </si>
   <si>
-    <t>Max LED current</t>
-  </si>
-  <si>
-    <t>Ind. LED current</t>
-  </si>
-  <si>
     <t>https://www.ebay.co.uk/itm/Single-Core-Stranded-12V-24V-Cable-Thin-Wall-Wire-All-AMP-Ratings-11-Colours/202598012265?hash=item2f2bc85569:m:mQAiFprfL-Q-ktfsgXUBiqA&amp;var=502669964960</t>
   </si>
   <si>
@@ -132,10 +105,82 @@
     <t>Variable resistor on the +V source to allow the user to dim the LEDs</t>
   </si>
   <si>
-    <t>Variable resistor</t>
-  </si>
-  <si>
     <t>https://www.ebay.co.uk/itm/16mm-Variable-Resistor-Potentiometer-Pot-Lin-Linear-Log-Logarithmic/283066568348?hash=item41e8150e9c:m:mrbu8mZa6OFzxxFsL1i5JRA</t>
+  </si>
+  <si>
+    <t>330 resistor (100 pk)</t>
+  </si>
+  <si>
+    <t>Switch (1 pk)</t>
+  </si>
+  <si>
+    <t>Variable resistor (1 pk)</t>
+  </si>
+  <si>
+    <t>Ind. LED current (mA)</t>
+  </si>
+  <si>
+    <t>Max LED current (mA)</t>
+  </si>
+  <si>
+    <t>X by X by X cube, X:</t>
+  </si>
+  <si>
+    <t>GPIO pins:</t>
+  </si>
+  <si>
+    <t>No. Needed</t>
+  </si>
+  <si>
+    <t>One 330 ohm resistor on each anode, X^2</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/1-27mm-Pitch-32-Inch-26-Pin-IDC-Flat-Ribbon-Cable-Connector-Multicolor/362590979279?epid=2098098999&amp;hash=item546c1b44cf:g:vOkAAOSw4NZcls72</t>
+  </si>
+  <si>
+    <t>Ribbon cable (26 pin)</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>LED (1000 pk)</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/3mm-5mm-10mm-Round-top-Diffused-Super-Bright-LED-light-lamp-Wholesale-DIY/161289178158?hash=item258d958c2e:m:m-dYiRP3M9W0CL2WXCIXOzw</t>
+  </si>
+  <si>
+    <t>Use diffused LEDs</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/10-x-1000uF-16V-105C-Radial-Electrolytic-Capacitor-10-x-13mm-Q7U7/183867763045?hash=item2acf5f6965:g:rl0AAOSwqsNdGpJg</t>
+  </si>
+  <si>
+    <t>1000uF Capacitors (10 pk)</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/20-x-100uF-16V-105C-Radial-Electrolytic-Capacitor-5x7mm-X8V2/173952174914?epid=2212232404&amp;hash=item28805b8b42:g:e~AAAOSwjxddG8dg</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/DC-3-3V-5V-9V-12V-18V-24V-36V-48V-Universal-Regulated-Switching-Power-Supply/151886747221?hash=item235d27d655:m:mMEkoTOvhjS1w4-JpB9s6Ag</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/50PCS-Transistor-MOT-ON-ST-FSC-TO-92-PN2222-PN2222A/273089920081?hash=item3f956d7c51:g:iCAAAOSwnF9Y6FyI</t>
+  </si>
+  <si>
+    <t>Transistors (50 pk)</t>
+  </si>
+  <si>
+    <t>5V 3A PSU</t>
+  </si>
+  <si>
+    <t>100uF Capacitors (20 pk)</t>
+  </si>
+  <si>
+    <t>GPIO Hat (16 pin)</t>
+  </si>
+  <si>
+    <t>https://www.abelectronics.co.uk/p/71/io-pi-zero</t>
   </si>
 </sst>
 </file>
@@ -148,7 +193,7 @@
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,6 +232,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -196,7 +249,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -373,6 +426,28 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -382,24 +457,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -414,36 +476,65 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="13" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -761,321 +852,485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7544310A-3F69-B748-89F1-389435FD61CD}">
-  <dimension ref="B1:I24"/>
+  <dimension ref="B1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+    <row r="1" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="7">
+        <f>SUM(G:G)</f>
+        <v>65.72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="22">
+        <v>5</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="23">
+        <f>C5*(C5+1)</f>
+        <v>30</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="5">
+        <f>H5*(C5^2)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="36" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="12">
-        <f>SUM(F:F)</f>
-        <v>36.68</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="J7" s="37"/>
+    </row>
+    <row r="8" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="I8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="14">
+        <v>11.93</v>
+      </c>
+      <c r="E9" s="16">
+        <f>C5^3</f>
+        <v>125</v>
+      </c>
+      <c r="F9" s="13">
+        <f>ROUNDUP(E9/1000,  0)</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="14">
+        <f>F9*D9</f>
+        <v>11.93</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="9">
+      <c r="J9" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="E10" s="17">
+        <f>C5^2</f>
+        <v>25</v>
+      </c>
+      <c r="F10" s="9">
+        <f>ROUNDUP(E10/100,  0)</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
+        <f>F10*D10</f>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="I10" s="31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
+      <c r="J10" s="32"/>
+    </row>
+    <row r="11" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1.19</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="19">
+        <f>E11</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="12">
+        <f>F11*D11</f>
+        <v>1.19</v>
+      </c>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="12">
+        <v>2.79</v>
+      </c>
+      <c r="E12" s="17">
+        <v>2</v>
+      </c>
+      <c r="F12" s="19">
+        <f t="shared" ref="F12:F16" si="0">E12</f>
+        <v>2</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" ref="G12:G18" si="1">F12*D12</f>
+        <v>5.58</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="35"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2.69</v>
+      </c>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="1"/>
+        <v>2.69</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="8">
-        <f>C5*(C5+1)</f>
-        <v>20</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="10">
-        <f>G5*(C5^3)</f>
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="27"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="20">
-        <v>5.99</v>
-      </c>
-      <c r="E9" s="18">
-        <f>ROUNDUP(($C$5^3)/100,  0)</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="20">
-        <f>E9*D9</f>
-        <v>5.99</v>
-      </c>
-      <c r="H9" s="14" t="s">
+      <c r="C14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12">
+        <v>6.75</v>
+      </c>
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="25"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="E15" s="17">
+        <v>1</v>
+      </c>
+      <c r="F15" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="1"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="25"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="17">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="E10" s="14">
-        <f>ROUNDUP(($C$5^2)/100,  0)</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="17">
-        <f>E10*D10</f>
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="17">
-        <v>1.19</v>
-      </c>
-      <c r="E11" s="14">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17">
-        <f>E11*D11</f>
-        <v>1.19</v>
-      </c>
-      <c r="H11" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="17">
-        <v>2.79</v>
-      </c>
-      <c r="E12" s="14">
-        <v>2</v>
-      </c>
-      <c r="F12" s="17">
-        <f t="shared" ref="F12:F16" si="0">E12*D12</f>
-        <v>5.58</v>
-      </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="17">
-        <v>2.69</v>
-      </c>
-      <c r="E13" s="14">
-        <v>2</v>
-      </c>
-      <c r="F13" s="17">
-        <f t="shared" si="0"/>
-        <v>5.38</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="17">
-        <v>6.75</v>
-      </c>
-      <c r="E14" s="14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="17">
-        <f t="shared" si="0"/>
-        <v>6.75</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="29"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="17">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="E15" s="14">
-        <v>1</v>
-      </c>
-      <c r="F15" s="17">
-        <f t="shared" si="0"/>
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="17">
+      <c r="D16" s="12">
         <v>1.39</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="17">
         <v>0</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="13"/>
-      <c r="D17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="13"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="13"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" s="13"/>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" s="13"/>
-      <c r="D21" s="3"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" s="13"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" s="13"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C24" s="13"/>
+      <c r="G16" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="12">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E17" s="17">
+        <f>C6</f>
+        <v>30</v>
+      </c>
+      <c r="F17" s="19">
+        <f>ROUNDUP(E17/50, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" si="1"/>
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="12">
+        <v>3.94</v>
+      </c>
+      <c r="E18" s="17">
+        <f>ROUNDUP(C6/26, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="19">
+        <f>E18</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="12">
+        <f t="shared" si="1"/>
+        <v>7.88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="E19" s="17">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" ref="G19:G22" si="2">F19*D19</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="2"/>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="12">
+        <v>5.79</v>
+      </c>
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1</v>
+      </c>
+      <c r="G21" s="12">
+        <f t="shared" si="2"/>
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="38">
+        <v>8.99</v>
+      </c>
+      <c r="E22" s="17">
+        <f>(MAX(0,ROUNDUP((C6-27)/16,0)))</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="19">
+        <f>E22</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="12">
+        <f t="shared" si="2"/>
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C23" s="8"/>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C24" s="8"/>
+      <c r="E24" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H13:I13"/>
+  <mergeCells count="9">
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="I10:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C9" r:id="rId1" xr:uid="{C5A6056E-C597-C342-A85E-C5B7015FDFDD}"/>
-    <hyperlink ref="C10" r:id="rId2" xr:uid="{1378F69A-0504-0F40-9AA0-C0B729490F04}"/>
-    <hyperlink ref="C11" r:id="rId3" xr:uid="{E0BFF44F-384A-4A4B-8728-C5FBBEF8767E}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{F77CEC88-1F87-4843-8FAB-D49099BCD838}"/>
-    <hyperlink ref="C13" r:id="rId5" xr:uid="{9F71FF18-DBC6-1C48-83A5-9D6CCFDE76F5}"/>
-    <hyperlink ref="C14" r:id="rId6" xr:uid="{0753A44B-EDA5-E043-A855-B8AB2428A7D5}"/>
-    <hyperlink ref="C15" r:id="rId7" xr:uid="{C9C04A39-A39C-2445-BF93-778AFF0C7D77}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{36EBF0B5-9C89-DB4A-9956-51E7A789055B}"/>
-    <hyperlink ref="I10" r:id="rId9" xr:uid="{08C09ECE-3146-CD4D-A704-3339D04E7071}"/>
-    <hyperlink ref="C16" r:id="rId10" xr:uid="{41A89E4C-1A4A-D542-9D20-2370BCCA3989}"/>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{1378F69A-0504-0F40-9AA0-C0B729490F04}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{E0BFF44F-384A-4A4B-8728-C5FBBEF8767E}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{F77CEC88-1F87-4843-8FAB-D49099BCD838}"/>
+    <hyperlink ref="C13" r:id="rId4" xr:uid="{9F71FF18-DBC6-1C48-83A5-9D6CCFDE76F5}"/>
+    <hyperlink ref="C14" r:id="rId5" xr:uid="{0753A44B-EDA5-E043-A855-B8AB2428A7D5}"/>
+    <hyperlink ref="C15" r:id="rId6" xr:uid="{C9C04A39-A39C-2445-BF93-778AFF0C7D77}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{36EBF0B5-9C89-DB4A-9956-51E7A789055B}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{08C09ECE-3146-CD4D-A704-3339D04E7071}"/>
+    <hyperlink ref="C16" r:id="rId9" xr:uid="{41A89E4C-1A4A-D542-9D20-2370BCCA3989}"/>
+    <hyperlink ref="C18" r:id="rId10" xr:uid="{CEFB5ED7-F0B5-024B-8AEC-DA005799A89F}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{D4CCB994-6DF0-4140-A228-422EC196BF88}"/>
+    <hyperlink ref="C19" r:id="rId12" xr:uid="{F5D8D916-C5D1-8D4B-8187-F9623C051F77}"/>
+    <hyperlink ref="C20" r:id="rId13" xr:uid="{A05EB672-EA40-E74A-9DCF-F604525F40BD}"/>
+    <hyperlink ref="C21" r:id="rId14" xr:uid="{E5956D78-6E91-6048-B22F-C569705524A6}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{1B695572-0F64-AB43-AA6C-0C26E3E3AFDB}"/>
+    <hyperlink ref="C22" r:id="rId16" xr:uid="{A3F2C4B6-2A1C-524D-8FE9-3363F3B9E421}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to use shift registers
</commit_message>
<xml_diff>
--- a/LED Cube Shopping list.xlsx
+++ b/LED Cube Shopping list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wild/Documents/Projects/trackellite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A262E69-38F3-4245-A5C5-15A51A53033B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D1273F-0ABF-BE42-AB8B-188A6C62E368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{4821D1B7-1E32-564A-9100-CE974E243A21}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Shopping list for LED cube</t>
   </si>
@@ -51,39 +53,9 @@
     <t>https://www.ebay.co.uk/itm/Resistor-Metal-Film-1-4W-0-25W-5-10-200-270-470-1k-3-3k-10k-20k-47k-Ohm/382625214567?hash=item59163d7067:m:msYdoHTiPmHJqz_OMMrQp8Q&amp;var=651378842494</t>
   </si>
   <si>
-    <t>Heat Shrink</t>
-  </si>
-  <si>
-    <t>https://www.ebay.co.uk/itm/Heat-Shrink-2-1-Tube-Tubing-Sleeve-Sleeving-Heat-Shrink-All-Colours-and-Sizes/261960089592?hash=item3cfe09bff8:m:m_EwYaXKVhKo0WUxKvmODIA</t>
-  </si>
-  <si>
-    <t>https://www.ebay.co.uk/itm/illuminated-LED-Toggle-Switch-With-Missile-Style-Flick-Cover-12V-Car-Dash/282258203997?hash=item41b7e6655d:m:mL95Oa7ssQttGbXRMt0rJ9A&amp;var=581300324809</t>
-  </si>
-  <si>
-    <t>https://www.ebay.co.uk/itm/Single-Core-Stranded-12V-24V-Cable-Thin-Wall-Wire-All-AMP-Ratings-11-Colours/202598012265?hash=item2f2bc85569:m:mQAiFprfL-Q-ktfsgXUBiqA&amp;var=502669964960</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Wire Stripper</t>
-  </si>
-  <si>
-    <t>https://www.ebay.co.uk/itm/Self-Adjustable-Automatic-Cable-Wire-Crimper-Crimping-Tool-Stripper-Plier-Cutter/401457846747?epid=16031184053&amp;hash=item5d78c099db:g:TSMAAOSwXCVcgmxi</t>
-  </si>
-  <si>
-    <t>Pi Zero W</t>
-  </si>
-  <si>
-    <t>https://thepihut.com/products/raspberry-pi-zero-w</t>
-  </si>
-  <si>
-    <t>LED Cube instructable. VERY handy</t>
-  </si>
-  <si>
-    <t>https://www.instructables.com/id/Led-Cube-8x8x8/</t>
-  </si>
-  <si>
     <t>How does an LED matrix work?</t>
   </si>
   <si>
@@ -96,27 +68,12 @@
     <t>Should I use transistors to switch the anodes? This way, I can isolate the control electronics from the (potentially beefy) LED driver current.</t>
   </si>
   <si>
-    <t>7A Wire</t>
-  </si>
-  <si>
     <t>7A wire is overkill for all but the biggest LED cubes, but it will help prop the structure up.</t>
   </si>
   <si>
     <t>Variable resistor on the +V source to allow the user to dim the LEDs</t>
   </si>
   <si>
-    <t>https://www.ebay.co.uk/itm/16mm-Variable-Resistor-Potentiometer-Pot-Lin-Linear-Log-Logarithmic/283066568348?hash=item41e8150e9c:m:mrbu8mZa6OFzxxFsL1i5JRA</t>
-  </si>
-  <si>
-    <t>330 resistor (100 pk)</t>
-  </si>
-  <si>
-    <t>Switch (1 pk)</t>
-  </si>
-  <si>
-    <t>Variable resistor (1 pk)</t>
-  </si>
-  <si>
     <t>Ind. LED current (mA)</t>
   </si>
   <si>
@@ -168,19 +125,22 @@
     <t>https://www.ebay.co.uk/itm/50PCS-Transistor-MOT-ON-ST-FSC-TO-92-PN2222-PN2222A/273089920081?hash=item3f956d7c51:g:iCAAAOSwnF9Y6FyI</t>
   </si>
   <si>
-    <t>Transistors (50 pk)</t>
-  </si>
-  <si>
     <t>5V 3A PSU</t>
   </si>
   <si>
     <t>100uF Capacitors (20 pk)</t>
   </si>
   <si>
-    <t>GPIO Hat (16 pin)</t>
-  </si>
-  <si>
-    <t>https://www.abelectronics.co.uk/p/71/io-pi-zero</t>
+    <t>330R resistor (100 pk)</t>
+  </si>
+  <si>
+    <t>PN222 Transistors (50 pk)</t>
+  </si>
+  <si>
+    <t>74HCT595 shift registers</t>
+  </si>
+  <si>
+    <t>https://www.bitsbox.co.uk/index.php?main_page=product_info&amp;cPath=140_158&amp;products_id=1171</t>
   </si>
 </sst>
 </file>
@@ -457,7 +417,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -534,7 +494,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -852,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7544310A-3F69-B748-89F1-389435FD61CD}">
-  <dimension ref="B1:J24"/>
+  <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,7 +839,7 @@
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
       <c r="E2" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -889,18 +848,18 @@
       <c r="D3" s="26"/>
       <c r="E3" s="7">
         <f>SUM(G:G)</f>
-        <v>65.72</v>
+        <v>41.260000000000005</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C5" s="22">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="G5" s="28"/>
       <c r="H5" s="4">
@@ -909,24 +868,24 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C6" s="23">
         <f>C5*(C5+1)</f>
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G6" s="30"/>
       <c r="H6" s="5">
         <f>H5*(C5^2)</f>
-        <v>500</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I7" s="36" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="J7" s="37"/>
     </row>
@@ -941,34 +900,34 @@
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D9" s="14">
         <v>11.93</v>
       </c>
       <c r="E9" s="16">
         <f>C5^3</f>
-        <v>125</v>
+        <v>512</v>
       </c>
       <c r="F9" s="13">
         <f>ROUNDUP(E9/1000,  0)</f>
@@ -978,16 +937,14 @@
         <f>F9*D9</f>
         <v>11.93</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="I9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>5</v>
@@ -997,7 +954,7 @@
       </c>
       <c r="E10" s="17">
         <f>C5^2</f>
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="F10" s="9">
         <f>ROUNDUP(E10/100,  0)</f>
@@ -1007,330 +964,187 @@
         <f>F10*D10</f>
         <v>2.4900000000000002</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="33"/>
+      <c r="J10" s="34"/>
+    </row>
+    <row r="11" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="12">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="E11" s="17">
+        <f>C6</f>
+        <v>72</v>
+      </c>
+      <c r="F11" s="19">
+        <f>ROUNDUP(E11/50, 0)</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" ref="G11:G13" si="0">F11*D11</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="35"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="32"/>
-    </row>
-    <row r="11" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="12">
-        <v>1.19</v>
-      </c>
-      <c r="E11" s="17">
-        <v>1</v>
-      </c>
-      <c r="F11" s="19">
-        <f>E11</f>
-        <v>1</v>
-      </c>
-      <c r="G11" s="12">
-        <f>F11*D11</f>
-        <v>1.19</v>
-      </c>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="12">
+        <v>3.94</v>
+      </c>
+      <c r="E12" s="17">
+        <f>ROUNDUP(C6/26, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="F12" s="19">
+        <f>E12</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="0"/>
+        <v>11.82</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="25"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E13" s="17">
+        <f>C5+1</f>
+        <v>9</v>
+      </c>
+      <c r="F13" s="19">
+        <f>E13</f>
+        <v>9</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="25"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="12">
-        <v>2.79</v>
-      </c>
-      <c r="E12" s="17">
-        <v>2</v>
-      </c>
-      <c r="F12" s="19">
-        <f t="shared" ref="F12:F16" si="0">E12</f>
-        <v>2</v>
-      </c>
-      <c r="G12" s="12">
-        <f t="shared" ref="G12:G18" si="1">F12*D12</f>
-        <v>5.58</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="35"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="12">
-        <v>2.69</v>
-      </c>
-      <c r="E13" s="17">
-        <v>1</v>
-      </c>
-      <c r="F13" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="12">
-        <f t="shared" si="1"/>
-        <v>2.69</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="25"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
+      <c r="C14" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="D14" s="12">
-        <v>6.75</v>
+        <v>0.99</v>
       </c>
       <c r="E14" s="17">
         <v>1</v>
       </c>
-      <c r="F14" s="19">
-        <f t="shared" si="0"/>
+      <c r="F14" s="9">
         <v>1</v>
       </c>
       <c r="G14" s="12">
-        <f t="shared" si="1"/>
-        <v>6.75</v>
+        <f t="shared" ref="G14:G16" si="1">F14*D14</f>
+        <v>0.99</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J14" s="25"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>14</v>
+      <c r="B15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D15" s="12">
-        <v>9.3000000000000007</v>
+        <v>0.99</v>
       </c>
       <c r="E15" s="17">
         <v>1</v>
       </c>
-      <c r="F15" s="19">
-        <f t="shared" si="0"/>
+      <c r="F15" s="9">
         <v>1</v>
       </c>
       <c r="G15" s="12">
         <f t="shared" si="1"/>
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="J15" s="25"/>
+        <v>0.99</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D16" s="12">
-        <v>1.39</v>
+        <v>5.79</v>
       </c>
       <c r="E16" s="17">
-        <v>0</v>
-      </c>
-      <c r="F16" s="19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
       </c>
       <c r="G16" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="12">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E17" s="17">
-        <f>C6</f>
-        <v>30</v>
-      </c>
-      <c r="F17" s="19">
-        <f>ROUNDUP(E17/50, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="G17" s="12">
-        <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="12">
-        <v>3.94</v>
-      </c>
-      <c r="E18" s="17">
-        <f>ROUNDUP(C6/26, 0)</f>
-        <v>2</v>
-      </c>
-      <c r="F18" s="19">
-        <f>E18</f>
-        <v>2</v>
-      </c>
-      <c r="G18" s="12">
-        <f t="shared" si="1"/>
-        <v>7.88</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0.99</v>
-      </c>
-      <c r="E19" s="17">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-      <c r="G19" s="12">
-        <f t="shared" ref="G19:G22" si="2">F19*D19</f>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0.99</v>
-      </c>
-      <c r="E20" s="17">
-        <v>1</v>
-      </c>
-      <c r="F20" s="9">
-        <v>1</v>
-      </c>
-      <c r="G20" s="12">
-        <f t="shared" si="2"/>
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="12">
         <v>5.79</v>
       </c>
-      <c r="E21" s="17">
-        <v>1</v>
-      </c>
-      <c r="F21" s="9">
-        <v>1</v>
-      </c>
-      <c r="G21" s="12">
-        <f t="shared" si="2"/>
-        <v>5.79</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="38">
-        <v>8.99</v>
-      </c>
-      <c r="E22" s="17">
-        <f>(MAX(0,ROUNDUP((C6-27)/16,0)))</f>
-        <v>1</v>
-      </c>
-      <c r="F22" s="19">
-        <f>E22</f>
-        <v>1</v>
-      </c>
-      <c r="G22" s="12">
-        <f t="shared" si="2"/>
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="8"/>
-      <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="8"/>
-      <c r="E24" s="18"/>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18" s="8"/>
+      <c r="E18" s="18"/>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="8"/>
+      <c r="E19" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I12:J12"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="I10:J11"/>
-    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="I7:J7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{1378F69A-0504-0F40-9AA0-C0B729490F04}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{E0BFF44F-384A-4A4B-8728-C5FBBEF8767E}"/>
-    <hyperlink ref="C12" r:id="rId3" xr:uid="{F77CEC88-1F87-4843-8FAB-D49099BCD838}"/>
-    <hyperlink ref="C13" r:id="rId4" xr:uid="{9F71FF18-DBC6-1C48-83A5-9D6CCFDE76F5}"/>
-    <hyperlink ref="C14" r:id="rId5" xr:uid="{0753A44B-EDA5-E043-A855-B8AB2428A7D5}"/>
-    <hyperlink ref="C15" r:id="rId6" xr:uid="{C9C04A39-A39C-2445-BF93-778AFF0C7D77}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{36EBF0B5-9C89-DB4A-9956-51E7A789055B}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{08C09ECE-3146-CD4D-A704-3339D04E7071}"/>
-    <hyperlink ref="C16" r:id="rId9" xr:uid="{41A89E4C-1A4A-D542-9D20-2370BCCA3989}"/>
-    <hyperlink ref="C18" r:id="rId10" xr:uid="{CEFB5ED7-F0B5-024B-8AEC-DA005799A89F}"/>
-    <hyperlink ref="C9" r:id="rId11" xr:uid="{D4CCB994-6DF0-4140-A228-422EC196BF88}"/>
-    <hyperlink ref="C19" r:id="rId12" xr:uid="{F5D8D916-C5D1-8D4B-8187-F9623C051F77}"/>
-    <hyperlink ref="C20" r:id="rId13" xr:uid="{A05EB672-EA40-E74A-9DCF-F604525F40BD}"/>
-    <hyperlink ref="C21" r:id="rId14" xr:uid="{E5956D78-6E91-6048-B22F-C569705524A6}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{1B695572-0F64-AB43-AA6C-0C26E3E3AFDB}"/>
-    <hyperlink ref="C22" r:id="rId16" xr:uid="{A3F2C4B6-2A1C-524D-8FE9-3363F3B9E421}"/>
+    <hyperlink ref="J8" r:id="rId2" xr:uid="{08C09ECE-3146-CD4D-A704-3339D04E7071}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{CEFB5ED7-F0B5-024B-8AEC-DA005799A89F}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{D4CCB994-6DF0-4140-A228-422EC196BF88}"/>
+    <hyperlink ref="C14" r:id="rId5" xr:uid="{F5D8D916-C5D1-8D4B-8187-F9623C051F77}"/>
+    <hyperlink ref="C15" r:id="rId6" xr:uid="{A05EB672-EA40-E74A-9DCF-F604525F40BD}"/>
+    <hyperlink ref="C16" r:id="rId7" xr:uid="{E5956D78-6E91-6048-B22F-C569705524A6}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{1B695572-0F64-AB43-AA6C-0C26E3E3AFDB}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{8EB23206-0EEE-E342-A212-BAE228936160}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>